<commit_message>
Import Kaizen upload Coding
</commit_message>
<xml_diff>
--- a/Kaizen.Web/wwwroot/assets/Template/sample_users.xlsx
+++ b/Kaizen.Web/wwwroot/assets/Template/sample_users.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$6</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,62 +39,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
-  <si>
-    <t>Emp NO</t>
-  </si>
-  <si>
-    <t>RESOURCE NAME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>EMAIL ID</t>
-  </si>
-  <si>
-    <t>DOMAIN</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
-    <t>Kanicka Mary D</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>Quality</t>
-  </si>
-  <si>
-    <t>Quality - Assembly</t>
-  </si>
-  <si>
-    <t>G.DINESHKUMAR</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>Quality - Metrology</t>
-  </si>
-  <si>
-    <t>GOWSHIK DHARAN U</t>
-  </si>
-  <si>
-    <t>HARISH M</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Engineering - Band</t>
-  </si>
-  <si>
-    <t>Moulidharan.C</t>
-  </si>
-  <si>
     <t>kanicka.*****@tataelectronics.co.in</t>
   </si>
   <si>
@@ -135,6 +93,75 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>DepartmentQ</t>
+  </si>
+  <si>
+    <t>Department6</t>
+  </si>
+  <si>
+    <t>Department3</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Emp Id</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Kanicka</t>
+  </si>
+  <si>
+    <t>GOWSHIK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mary </t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>G.DINESH</t>
+  </si>
+  <si>
+    <t>KUMAR</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DHARAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARISH </t>
+  </si>
+  <si>
+    <t>Moulidharan.</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -189,12 +216,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -236,22 +269,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -264,37 +298,7 @@
     <cellStyle name="Normal 7" xfId="5"/>
     <cellStyle name="Normal 9" xfId="6"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -352,13 +356,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>617061</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>42048</xdr:rowOff>
@@ -413,13 +417,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>463550</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1066466</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>148898</xdr:rowOff>
@@ -776,184 +780,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2">
+        <v>9899140569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2">
+        <v>9899140570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2">
+        <v>9899140571</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9899140572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="G6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>29</v>
+      <c r="J6" s="2">
+        <v>9899140573</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D6">
-    <cfRule type="duplicateValues" dxfId="6" priority="1021"/>
+  <conditionalFormatting sqref="F1:F6">
+    <cfRule type="duplicateValues" dxfId="3" priority="1021"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6">
-    <cfRule type="duplicateValues" dxfId="5" priority="1022"/>
+  <conditionalFormatting sqref="A1:A6 C1:C6">
+    <cfRule type="duplicateValues" dxfId="2" priority="1022"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6">
-    <cfRule type="duplicateValues" dxfId="4" priority="1023"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6">
-    <cfRule type="duplicateValues" dxfId="3" priority="1024"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="1025"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6">
-    <cfRule type="duplicateValues" dxfId="1" priority="1026"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1027"/>
+  <conditionalFormatting sqref="A1:A6 C1:C6">
+    <cfRule type="duplicateValues" dxfId="1" priority="1024"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1025"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
View User Screen - Added New Column Block in Bulk User Upload (Import Kaizen) .
</commit_message>
<xml_diff>
--- a/Kaizen.Web/wwwroot/assets/Template/sample_users.xlsx
+++ b/Kaizen.Web/wwwroot/assets/Template/sample_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manas Kumar Lenka\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$6</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Gender</t>
   </si>
@@ -95,21 +95,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>DepartmentQ</t>
-  </si>
-  <si>
-    <t>Department6</t>
-  </si>
-  <si>
-    <t>Department3</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Emp Id</t>
   </si>
   <si>
@@ -162,6 +147,27 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Testing121</t>
+  </si>
+  <si>
+    <t>Department1204</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>departmentviswa123</t>
+  </si>
+  <si>
+    <t>Block 4</t>
   </si>
 </sst>
 </file>
@@ -780,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,55 +800,59 @@
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>33</v>
+      <c r="K1" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
@@ -851,29 +861,34 @@
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>9899140569</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
@@ -881,30 +896,33 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>9899140570</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
@@ -913,24 +931,27 @@
         <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>9899140571</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
@@ -943,28 +964,31 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>9899140572</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
@@ -973,20 +997,23 @@
         <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>9899140573</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F6">
+  <conditionalFormatting sqref="F1:G1 F2:F6">
     <cfRule type="duplicateValues" dxfId="3" priority="1021"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A6 C1:C6">
@@ -997,11 +1024,11 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1025"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Removed Middle Name from Import Kaizen upload .
</commit_message>
<xml_diff>
--- a/Kaizen.Web/wwwroot/assets/Template/sample_users.xlsx
+++ b/Kaizen.Web/wwwroot/assets/Template/sample_users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manas Kumar Lenka\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$6</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Gender</t>
   </si>
@@ -101,9 +101,6 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>GOWSHIK</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mary </t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -131,13 +125,7 @@
     <t>G.DINESH</t>
   </si>
   <si>
-    <t>KUMAR</t>
-  </si>
-  <si>
     <t>U</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DHARAN </t>
   </si>
   <si>
     <t xml:space="preserve">HARISH </t>
@@ -362,13 +350,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>617061</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>42048</xdr:rowOff>
@@ -423,13 +411,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>463550</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1066466</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>148898</xdr:rowOff>
@@ -786,27 +774,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.6328125" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -817,218 +804,204 @@
         <v>20</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2">
+      <c r="J2" s="2">
         <v>9899140569</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" s="2">
         <v>9899140570</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="2">
+      <c r="J4" s="2">
         <v>9899140571</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="2">
+      <c r="J5" s="2">
         <v>9899140572</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="2">
+      <c r="J6" s="2">
         <v>9899140573</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:G1 F2:F6">
+  <conditionalFormatting sqref="E1:F1 E2:E6">
     <cfRule type="duplicateValues" dxfId="3" priority="1021"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6 C1:C6">
-    <cfRule type="duplicateValues" dxfId="2" priority="1022"/>
+  <conditionalFormatting sqref="A1:A6">
+    <cfRule type="duplicateValues" dxfId="2" priority="1027"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6 C1:C6">
-    <cfRule type="duplicateValues" dxfId="1" priority="1024"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1025"/>
+  <conditionalFormatting sqref="A1:A6">
+    <cfRule type="duplicateValues" dxfId="1" priority="1028"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1029"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F2" r:id="rId5"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>